<commit_message>
Script DataFrames Auxiliares Creado
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/FacturasPAMI.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/FacturasPAMI.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\facoep\Sistemas\Agustin\Reportes BI\2021\Facturación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Facturas PAMI 2020" sheetId="1" r:id="rId1"/>
     <sheet name="Facturas PAMI 2021" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,12 +54,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;XDR&quot;* #,##0.00_-;\-&quot;XDR&quot;* #,##0.00_-;_-&quot;XDR&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -116,22 +116,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -418,17 +418,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -787,7 +788,7 @@
         <v>78936637</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:D22" si="0">C14-SUM(E14:H14)</f>
+        <f t="shared" ref="D14:D30" si="0">C14-SUM(E14:H14)</f>
         <v>82300335.340000004</v>
       </c>
       <c r="E14" s="2">
@@ -1024,7 +1025,225 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="A23" s="8">
+        <v>44200</v>
+      </c>
+      <c r="B23" s="1">
+        <v>13222</v>
+      </c>
+      <c r="C23" s="2">
+        <v>78444711.159999996</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>85848557.829999998</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2526120.0499999998</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>-227540.65</v>
+      </c>
+      <c r="H23" s="2">
+        <f>-9696292.58-6133.49</f>
+        <v>-9702426.0700000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>44228</v>
+      </c>
+      <c r="B24" s="1">
+        <v>13916</v>
+      </c>
+      <c r="C24" s="2">
+        <v>82646023.120000005</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>90113341.210000008</v>
+      </c>
+      <c r="E24" s="2">
+        <v>999772.3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1715.7</v>
+      </c>
+      <c r="G24" s="2">
+        <f>-204072.27-4827.88</f>
+        <v>-208900.15</v>
+      </c>
+      <c r="H24" s="2">
+        <f>-7664309.47-595596.47</f>
+        <v>-8259905.9399999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>44256</v>
+      </c>
+      <c r="B25" s="1">
+        <v>14756</v>
+      </c>
+      <c r="C25" s="2">
+        <v>84682969.269999996</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>90275048.36999999</v>
+      </c>
+      <c r="E25" s="2">
+        <v>918376.51</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1205.72</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-192486.41</v>
+      </c>
+      <c r="H25" s="2">
+        <v>-6319174.9199999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>44292</v>
+      </c>
+      <c r="B26" s="1">
+        <v>15523</v>
+      </c>
+      <c r="C26" s="2">
+        <v>85617373.560000002</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>95466150.359999999</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1505471.18</v>
+      </c>
+      <c r="F26" s="2">
+        <v>18200.66</v>
+      </c>
+      <c r="G26" s="2">
+        <v>-273730.84999999998</v>
+      </c>
+      <c r="H26" s="2">
+        <v>-11098717.789999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>44319</v>
+      </c>
+      <c r="B27" s="1">
+        <v>16334</v>
+      </c>
+      <c r="C27" s="2">
+        <v>87512251.659999996</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>95886049.890000001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1484598.43</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5778.78</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-233094.29</v>
+      </c>
+      <c r="H27" s="2">
+        <v>-9631081.1500000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>44348</v>
+      </c>
+      <c r="B28" s="1">
+        <v>88196</v>
+      </c>
+      <c r="C28" s="2">
+        <f>77514763.83+21243509.85</f>
+        <v>98758273.680000007</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>105594983.59</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2239762.44</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1041.93</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-245940.37</v>
+      </c>
+      <c r="H28" s="2">
+        <v>-8831573.9100000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>44378</v>
+      </c>
+      <c r="B29" s="1">
+        <v>156474</v>
+      </c>
+      <c r="C29" s="2">
+        <v>106853801.95</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>112914883.12</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4347264.2300000004</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1890.9</v>
+      </c>
+      <c r="G29" s="2">
+        <v>-280692.21000000002</v>
+      </c>
+      <c r="H29" s="2">
+        <v>-10129544.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B30" s="1">
+        <v>421851</v>
+      </c>
+      <c r="C30" s="2">
+        <f>83853447.67+21686755.93</f>
+        <v>105540203.59999999</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>122936905.19999999</v>
+      </c>
+      <c r="E30" s="9">
+        <v>3230463.38</v>
+      </c>
+      <c r="F30" s="2">
+        <v>9028.9</v>
+      </c>
+      <c r="G30" s="2">
+        <v>-452225.06</v>
+      </c>
+      <c r="H30" s="2">
+        <v>-20183968.82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1036,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>